<commit_message>
Fix Playwright asyncio loop error for multi-color processing
The Playwright instance was created in login() but never stopped when
close() was called. This left the asyncio event loop active, causing
"asyncio loop" errors when processing subsequent colors.

Changes:
- Store Playwright instance as self._playwright in __init__
- Stop Playwright instance in close() before closing browser
- Verified fix by successfully processing all 18 colors without errors

Result:
- First color: Login succeeds
- All subsequent colors: Login succeeds (no asyncio errors)
- Product generated: 72 variants, 184 images with correct alt tags

🤖 Generated with [Claude Code](https://claude.com/claude-code)

Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/purinamills/input/purina-mills.xlsx
+++ b/purinamills/input/purina-mills.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11102"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/moosemarketer/Code/Python/collectors/purinamills/input/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/moosemarketer/Code/garoppos/collectors/purinamills/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E13B6C1-51D3-1C4F-9C1F-9C6FFF6A5AFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{092037D1-FC33-D240-97C3-72B161BA5B0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="160" yWindow="660" windowWidth="17680" windowHeight="20500" xr2:uid="{E6343A4B-923C-2A4F-A319-EF0629843702}"/>
+    <workbookView xWindow="36000" yWindow="1460" windowWidth="38080" windowHeight="20780" xr2:uid="{E6343A4B-923C-2A4F-A319-EF0629843702}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -3288,9 +3288,6 @@
     <t>2 LB</t>
   </si>
   <si>
-    <t>3 - 0.17 PACKETS</t>
-  </si>
-  <si>
     <t>1 GALLON</t>
   </si>
   <si>
@@ -3511,6 +3508,9 @@
   </si>
   <si>
     <t>color</t>
+  </si>
+  <si>
+    <t>3 - 0.17 OZ PACKETS</t>
   </si>
 </sst>
 </file>
@@ -3918,8 +3918,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB9C2E4C-43DE-1149-9743-AA8FD8D35C0A}">
   <dimension ref="A1:AX63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AX1" workbookViewId="0">
-      <selection activeCell="AX1" sqref="AX1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F1" sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -3935,7 +3935,7 @@
     <col min="12" max="12" width="21.5703125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="7" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="7" customWidth="1"/>
-    <col min="15" max="15" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="18.140625" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="27.7109375" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="27.28515625" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="8.140625" bestFit="1" customWidth="1"/>
@@ -3985,19 +3985,19 @@
         <v>1032</v>
       </c>
       <c r="E1" s="2" t="s">
+        <v>1151</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>1152</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>1153</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>1154</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>1155</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>1156</v>
       </c>
       <c r="J1" s="2" t="s">
         <v>1033</v>
@@ -4012,7 +4012,7 @@
         <v>1036</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>1157</v>
+        <v>1156</v>
       </c>
       <c r="O1" s="2" t="s">
         <v>1037</v>
@@ -4138,7 +4138,7 @@
         <v>2</v>
       </c>
       <c r="J2" t="s">
-        <v>1094</v>
+        <v>1093</v>
       </c>
       <c r="K2" s="1" t="s">
         <v>3</v>
@@ -4247,7 +4247,7 @@
         <v>2</v>
       </c>
       <c r="J3" t="s">
-        <v>1095</v>
+        <v>1094</v>
       </c>
       <c r="K3" s="1" t="s">
         <v>3</v>
@@ -4326,7 +4326,7 @@
         <v>2</v>
       </c>
       <c r="J4" t="s">
-        <v>1096</v>
+        <v>1095</v>
       </c>
       <c r="K4" s="1" t="s">
         <v>3</v>
@@ -4408,7 +4408,7 @@
         <v>2</v>
       </c>
       <c r="J5" t="s">
-        <v>1097</v>
+        <v>1096</v>
       </c>
       <c r="K5" s="1" t="s">
         <v>3</v>
@@ -4514,7 +4514,7 @@
         <v>2</v>
       </c>
       <c r="J6" t="s">
-        <v>1098</v>
+        <v>1097</v>
       </c>
       <c r="K6" s="1" t="s">
         <v>3</v>
@@ -4626,7 +4626,7 @@
         <v>2</v>
       </c>
       <c r="J7" t="s">
-        <v>1099</v>
+        <v>1098</v>
       </c>
       <c r="K7" s="1" t="s">
         <v>3</v>
@@ -4729,7 +4729,7 @@
         <v>2</v>
       </c>
       <c r="J8" t="s">
-        <v>1100</v>
+        <v>1099</v>
       </c>
       <c r="K8" s="1" t="s">
         <v>3</v>
@@ -4835,7 +4835,7 @@
         <v>2</v>
       </c>
       <c r="J9" t="s">
-        <v>1101</v>
+        <v>1100</v>
       </c>
       <c r="K9" s="1" t="s">
         <v>3</v>
@@ -4950,7 +4950,7 @@
         <v>2</v>
       </c>
       <c r="J10" t="s">
-        <v>1102</v>
+        <v>1101</v>
       </c>
       <c r="K10" s="1" t="s">
         <v>3</v>
@@ -5062,7 +5062,7 @@
         <v>2</v>
       </c>
       <c r="J11" t="s">
-        <v>1103</v>
+        <v>1102</v>
       </c>
       <c r="K11" s="1" t="s">
         <v>3</v>
@@ -5165,7 +5165,7 @@
         <v>2</v>
       </c>
       <c r="J12" t="s">
-        <v>1104</v>
+        <v>1103</v>
       </c>
       <c r="K12" s="1" t="s">
         <v>3</v>
@@ -5268,7 +5268,7 @@
         <v>2</v>
       </c>
       <c r="J13" t="s">
-        <v>1105</v>
+        <v>1104</v>
       </c>
       <c r="K13" s="1" t="s">
         <v>3</v>
@@ -5377,7 +5377,7 @@
         <v>2</v>
       </c>
       <c r="J14" t="s">
-        <v>1106</v>
+        <v>1105</v>
       </c>
       <c r="K14" s="1" t="s">
         <v>3</v>
@@ -5489,7 +5489,7 @@
         <v>2</v>
       </c>
       <c r="J15" t="s">
-        <v>1107</v>
+        <v>1106</v>
       </c>
       <c r="K15" s="1" t="s">
         <v>3</v>
@@ -5583,7 +5583,7 @@
         <v>2</v>
       </c>
       <c r="J16" t="s">
-        <v>1108</v>
+        <v>1107</v>
       </c>
       <c r="K16" s="1" t="s">
         <v>3</v>
@@ -5689,7 +5689,7 @@
         <v>2</v>
       </c>
       <c r="J17" t="s">
-        <v>1109</v>
+        <v>1108</v>
       </c>
       <c r="K17" s="1" t="s">
         <v>3</v>
@@ -5798,7 +5798,7 @@
         <v>2</v>
       </c>
       <c r="J18" t="s">
-        <v>1110</v>
+        <v>1109</v>
       </c>
       <c r="K18" s="1" t="s">
         <v>3</v>
@@ -5907,7 +5907,7 @@
         <v>2</v>
       </c>
       <c r="J19" t="s">
-        <v>1111</v>
+        <v>1110</v>
       </c>
       <c r="K19" s="1" t="s">
         <v>3</v>
@@ -6007,7 +6007,7 @@
         <v>2</v>
       </c>
       <c r="J20" t="s">
-        <v>1112</v>
+        <v>1111</v>
       </c>
       <c r="K20" s="1" t="s">
         <v>3</v>
@@ -6107,7 +6107,7 @@
         <v>2</v>
       </c>
       <c r="J21" t="s">
-        <v>1113</v>
+        <v>1112</v>
       </c>
       <c r="K21" s="1" t="s">
         <v>3</v>
@@ -6192,7 +6192,7 @@
         <v>2</v>
       </c>
       <c r="J22" t="s">
-        <v>1114</v>
+        <v>1113</v>
       </c>
       <c r="K22" s="1" t="s">
         <v>3</v>
@@ -6304,7 +6304,7 @@
         <v>1037</v>
       </c>
       <c r="J23" t="s">
-        <v>1115</v>
+        <v>1114</v>
       </c>
       <c r="K23" s="1" t="s">
         <v>3</v>
@@ -6313,7 +6313,7 @@
         <v>401</v>
       </c>
       <c r="O23" t="s">
-        <v>1084</v>
+        <v>1083</v>
       </c>
       <c r="P23" t="s">
         <v>402</v>
@@ -6419,13 +6419,13 @@
         <v>1037</v>
       </c>
       <c r="J24" t="s">
-        <v>1115</v>
+        <v>1114</v>
       </c>
       <c r="K24" s="1" t="s">
         <v>3</v>
       </c>
       <c r="O24" t="s">
-        <v>1085</v>
+        <v>1084</v>
       </c>
       <c r="P24" t="s">
         <v>419</v>
@@ -6522,7 +6522,7 @@
         <v>2</v>
       </c>
       <c r="J25" t="s">
-        <v>1116</v>
+        <v>1115</v>
       </c>
       <c r="K25" s="1" t="s">
         <v>3</v>
@@ -6610,7 +6610,7 @@
         <v>2</v>
       </c>
       <c r="J26" t="s">
-        <v>1117</v>
+        <v>1116</v>
       </c>
       <c r="K26" s="1" t="s">
         <v>3</v>
@@ -6701,7 +6701,7 @@
         <v>2</v>
       </c>
       <c r="J27" t="s">
-        <v>1118</v>
+        <v>1117</v>
       </c>
       <c r="K27" s="1" t="s">
         <v>3</v>
@@ -6813,7 +6813,7 @@
         <v>2</v>
       </c>
       <c r="J28" t="s">
-        <v>1119</v>
+        <v>1118</v>
       </c>
       <c r="K28" s="1" t="s">
         <v>3</v>
@@ -6916,7 +6916,7 @@
         <v>2</v>
       </c>
       <c r="J29" t="s">
-        <v>1120</v>
+        <v>1119</v>
       </c>
       <c r="K29" s="1" t="s">
         <v>3</v>
@@ -7025,7 +7025,7 @@
         <v>1037</v>
       </c>
       <c r="J30" t="s">
-        <v>1121</v>
+        <v>1120</v>
       </c>
       <c r="K30" s="1" t="s">
         <v>3</v>
@@ -7137,7 +7137,7 @@
         <v>1037</v>
       </c>
       <c r="J31" t="s">
-        <v>1121</v>
+        <v>1120</v>
       </c>
       <c r="K31" s="1" t="s">
         <v>3</v>
@@ -7243,7 +7243,7 @@
         <v>2</v>
       </c>
       <c r="J32" t="s">
-        <v>1122</v>
+        <v>1121</v>
       </c>
       <c r="K32" s="1" t="s">
         <v>3</v>
@@ -7358,13 +7358,13 @@
         <v>2</v>
       </c>
       <c r="J33" t="s">
-        <v>1123</v>
+        <v>1122</v>
       </c>
       <c r="K33" s="1" t="s">
         <v>3</v>
       </c>
       <c r="O33" t="s">
-        <v>1086</v>
+        <v>1085</v>
       </c>
       <c r="P33" t="s">
         <v>571</v>
@@ -7464,7 +7464,7 @@
         <v>2</v>
       </c>
       <c r="J34" t="s">
-        <v>1124</v>
+        <v>1123</v>
       </c>
       <c r="K34" s="1" t="s">
         <v>3</v>
@@ -7576,7 +7576,7 @@
         <v>2</v>
       </c>
       <c r="J35" t="s">
-        <v>1125</v>
+        <v>1124</v>
       </c>
       <c r="K35" s="1" t="s">
         <v>3</v>
@@ -7685,7 +7685,7 @@
         <v>2</v>
       </c>
       <c r="J36" t="s">
-        <v>1126</v>
+        <v>1125</v>
       </c>
       <c r="K36" s="1" t="s">
         <v>3</v>
@@ -7767,7 +7767,7 @@
         <v>2</v>
       </c>
       <c r="J37" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
       <c r="K37" s="1" t="s">
         <v>3</v>
@@ -7873,7 +7873,7 @@
         <v>2</v>
       </c>
       <c r="J38" t="s">
-        <v>1128</v>
+        <v>1127</v>
       </c>
       <c r="K38" s="1" t="s">
         <v>3</v>
@@ -7976,7 +7976,7 @@
         <v>2</v>
       </c>
       <c r="J39" t="s">
-        <v>1129</v>
+        <v>1128</v>
       </c>
       <c r="K39" s="1" t="s">
         <v>3</v>
@@ -8076,7 +8076,7 @@
         <v>2</v>
       </c>
       <c r="J40" t="s">
-        <v>1130</v>
+        <v>1129</v>
       </c>
       <c r="K40" s="1" t="s">
         <v>3</v>
@@ -8182,7 +8182,7 @@
         <v>2</v>
       </c>
       <c r="J41" t="s">
-        <v>1131</v>
+        <v>1130</v>
       </c>
       <c r="K41" s="1" t="s">
         <v>3</v>
@@ -8285,7 +8285,7 @@
         <v>2</v>
       </c>
       <c r="J42" t="s">
-        <v>1132</v>
+        <v>1131</v>
       </c>
       <c r="K42" s="1" t="s">
         <v>3</v>
@@ -8391,7 +8391,7 @@
         <v>2</v>
       </c>
       <c r="J43" t="s">
-        <v>1133</v>
+        <v>1132</v>
       </c>
       <c r="K43" s="1" t="s">
         <v>3</v>
@@ -8500,7 +8500,7 @@
         <v>2</v>
       </c>
       <c r="J44" t="s">
-        <v>1134</v>
+        <v>1133</v>
       </c>
       <c r="K44" s="1" t="s">
         <v>3</v>
@@ -8606,13 +8606,13 @@
         <v>2</v>
       </c>
       <c r="J45" t="s">
-        <v>1135</v>
+        <v>1134</v>
       </c>
       <c r="K45" s="1" t="s">
         <v>3</v>
       </c>
       <c r="O45" t="s">
-        <v>1083</v>
+        <v>1157</v>
       </c>
       <c r="P45" t="s">
         <v>751</v>
@@ -8703,7 +8703,7 @@
         <v>2</v>
       </c>
       <c r="J46" t="s">
-        <v>1136</v>
+        <v>1135</v>
       </c>
       <c r="K46" s="1" t="s">
         <v>3</v>
@@ -8779,7 +8779,7 @@
         <v>2</v>
       </c>
       <c r="J47" t="s">
-        <v>1137</v>
+        <v>1136</v>
       </c>
       <c r="K47" s="1" t="s">
         <v>3</v>
@@ -8858,7 +8858,7 @@
         <v>2</v>
       </c>
       <c r="J48" t="s">
-        <v>1138</v>
+        <v>1137</v>
       </c>
       <c r="K48" s="1" t="s">
         <v>3</v>
@@ -8967,7 +8967,7 @@
         <v>1037</v>
       </c>
       <c r="J49" t="s">
-        <v>1139</v>
+        <v>1138</v>
       </c>
       <c r="K49" s="1" t="s">
         <v>3</v>
@@ -9076,7 +9076,7 @@
         <v>1037</v>
       </c>
       <c r="J50" t="s">
-        <v>1139</v>
+        <v>1138</v>
       </c>
       <c r="K50" s="1" t="s">
         <v>3</v>
@@ -9179,7 +9179,7 @@
         <v>2</v>
       </c>
       <c r="J51" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
       <c r="K51" s="1" t="s">
         <v>3</v>
@@ -9258,7 +9258,7 @@
         <v>2</v>
       </c>
       <c r="J52" t="s">
-        <v>1141</v>
+        <v>1140</v>
       </c>
       <c r="K52" s="1" t="s">
         <v>3</v>
@@ -9376,7 +9376,7 @@
         <v>1037</v>
       </c>
       <c r="J53" t="s">
-        <v>1142</v>
+        <v>1141</v>
       </c>
       <c r="K53" s="1" t="s">
         <v>3</v>
@@ -9488,7 +9488,7 @@
         <v>1037</v>
       </c>
       <c r="J54" t="s">
-        <v>1142</v>
+        <v>1141</v>
       </c>
       <c r="K54" s="1" t="s">
         <v>3</v>
@@ -9597,7 +9597,7 @@
         <v>2</v>
       </c>
       <c r="J55" t="s">
-        <v>1143</v>
+        <v>1142</v>
       </c>
       <c r="K55" s="1" t="s">
         <v>3</v>
@@ -9700,7 +9700,7 @@
         <v>2</v>
       </c>
       <c r="J56" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="K56" s="1" t="s">
         <v>3</v>
@@ -9815,7 +9815,7 @@
         <v>2</v>
       </c>
       <c r="J57" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
       <c r="K57" s="1" t="s">
         <v>3</v>
@@ -9930,7 +9930,7 @@
         <v>2</v>
       </c>
       <c r="J58" t="s">
-        <v>1146</v>
+        <v>1145</v>
       </c>
       <c r="K58" s="1" t="s">
         <v>3</v>
@@ -10039,7 +10039,7 @@
         <v>2</v>
       </c>
       <c r="J59" t="s">
-        <v>1147</v>
+        <v>1146</v>
       </c>
       <c r="K59" s="1" t="s">
         <v>3</v>
@@ -10145,7 +10145,7 @@
         <v>2</v>
       </c>
       <c r="J60" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
       <c r="K60" s="1" t="s">
         <v>3</v>
@@ -10251,7 +10251,7 @@
         <v>2</v>
       </c>
       <c r="J61" t="s">
-        <v>1149</v>
+        <v>1148</v>
       </c>
       <c r="K61" s="1" t="s">
         <v>3</v>
@@ -10363,7 +10363,7 @@
         <v>2</v>
       </c>
       <c r="J62" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
       <c r="K62" s="1" t="s">
         <v>3</v>
@@ -10450,25 +10450,25 @@
     </row>
     <row r="63" spans="1:50">
       <c r="A63" t="s">
+        <v>1086</v>
+      </c>
+      <c r="B63" t="s">
         <v>1087</v>
-      </c>
-      <c r="B63" t="s">
-        <v>1088</v>
       </c>
       <c r="D63" t="s">
         <v>2</v>
       </c>
       <c r="J63" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="K63" s="1" t="s">
         <v>3</v>
       </c>
       <c r="O63" t="s">
+        <v>1088</v>
+      </c>
+      <c r="Q63" t="s">
         <v>1089</v>
-      </c>
-      <c r="Q63" t="s">
-        <v>1090</v>
       </c>
       <c r="V63" t="s">
         <v>420</v>
@@ -10498,16 +10498,16 @@
         <v>420</v>
       </c>
       <c r="AE63" t="s">
-        <v>1091</v>
+        <v>1090</v>
       </c>
       <c r="AF63" t="s">
         <v>76</v>
       </c>
       <c r="AG63" t="s">
+        <v>1091</v>
+      </c>
+      <c r="AH63" t="s">
         <v>1092</v>
-      </c>
-      <c r="AH63" t="s">
-        <v>1093</v>
       </c>
       <c r="AJ63" t="str">
         <f t="shared" si="4"/>

</xml_diff>